<commit_message>
Upload JS 10_Tugas & JS 11_Praktikum 1 dan Tugas_Perubahan
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FF8DCB-50E4-44F8-8389-0F6CEA1E76B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEA4426-6997-47A7-95D3-8D259746193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="12" windowWidth="23004" windowHeight="12948" xr2:uid="{D79EE337-E5BC-43E7-8244-EFA639F12D15}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D79EE337-E5BC-43E7-8244-EFA639F12D15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>kategori_id</t>
   </si>
   <si>
-    <t>barang_id</t>
-  </si>
-  <si>
     <t>barang_nama</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>MNM-004</t>
+  </si>
+  <si>
+    <t>barang_kode</t>
   </si>
 </sst>
 </file>
@@ -458,13 +458,13 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
@@ -475,16 +475,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -492,10 +492,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>22000</v>
@@ -509,10 +509,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>11500</v>
@@ -526,10 +526,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <v>17500</v>
@@ -543,10 +543,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>89000</v>
@@ -560,10 +560,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
         <v>3750</v>

</xml_diff>